<commit_message>
Update using actual births
</commit_message>
<xml_diff>
--- a/packages/processing/docs/Ziekenhuislocaties.xlsx
+++ b/packages/processing/docs/Ziekenhuislocaties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\web\vws\ziekenhuizen\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\home\erik\dev\test_ziekenhuizen\packages\processing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FFE31B-C5FA-429C-ACDE-A4D83B1C3409}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADAC26B-27E9-40EB-AF4D-BE4F2C3AAB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adressen SEH en AV" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="489">
   <si>
     <t>plaats</t>
   </si>
@@ -1486,18 +1486,37 @@
   </si>
   <si>
     <t>filename</t>
+  </si>
+  <si>
+    <t>bevallingen</t>
+  </si>
+  <si>
+    <t>perc2lLijnZh</t>
+  </si>
+  <si>
+    <t>perc1lLijnZh</t>
+  </si>
+  <si>
+    <t>perc1lLijnThuis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1508,12 +1527,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1548,8 +1561,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1560,6 +1587,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1602,22 +1634,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1630,8 +1662,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
@@ -2080,37 +2122,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O90"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A90"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="68" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.33203125" style="2"/>
+    <col min="2" max="2" width="31.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" style="2" customWidth="1"/>
+    <col min="14" max="15" width="12" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>475</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2128,7 +2173,7 @@
       <c r="H1" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>390</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -2140,15 +2185,27 @@
       <c r="L1" s="1" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -2166,7 +2223,7 @@
       <c r="H2" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="10" t="b">
+      <c r="I2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="5" t="b">
@@ -2178,15 +2235,27 @@
       <c r="L2" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M2" s="18">
+        <v>1608</v>
+      </c>
+      <c r="N2" s="16">
+        <v>0.79850746268656714</v>
+      </c>
+      <c r="O2" s="16">
+        <v>0.10261194029850747</v>
+      </c>
+      <c r="P2" s="16">
+        <v>9.8880597014925367E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>135</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -2204,7 +2273,7 @@
       <c r="H3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="10" t="b">
+      <c r="I3" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="5" t="b">
@@ -2216,15 +2285,27 @@
       <c r="L3" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M3" s="18">
+        <v>1764</v>
+      </c>
+      <c r="N3" s="16">
+        <v>0.68367346938775508</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0.11848072562358276</v>
+      </c>
+      <c r="P3" s="16">
+        <v>0.19784580498866214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>421</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2242,7 +2323,7 @@
       <c r="H4" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="10" t="b">
+      <c r="I4" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J4" s="5" t="b">
@@ -2254,15 +2335,27 @@
       <c r="L4" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M4" s="18">
+        <v>2847</v>
+      </c>
+      <c r="N4" s="16">
+        <v>0.74745345978222688</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0.12820512820512819</v>
+      </c>
+      <c r="P4" s="16">
+        <v>0.12434141201264488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>431</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>282</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -2280,7 +2373,7 @@
       <c r="H5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="10" t="b">
+      <c r="I5" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="5" t="b">
@@ -2292,15 +2385,27 @@
       <c r="L5" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M5" s="18">
+        <v>1852</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0.63336933045356369</v>
+      </c>
+      <c r="O5" s="16">
+        <v>0.18628509719222464</v>
+      </c>
+      <c r="P5" s="16">
+        <v>0.18034557235421167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>266</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2318,7 +2423,7 @@
       <c r="H6" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="10" t="b">
+      <c r="I6" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="5" t="b">
@@ -2330,16 +2435,27 @@
       <c r="L6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M6" s="18">
+        <v>1507</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0.85666887856668883</v>
+      </c>
+      <c r="O6" s="16">
+        <v>6.9011280690112808E-2</v>
+      </c>
+      <c r="P6" s="16">
+        <v>7.4319840743198404E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>417</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -2357,7 +2473,7 @@
       <c r="H7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="10" t="b">
+      <c r="I7" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="5" t="b">
@@ -2366,19 +2482,22 @@
       <c r="K7" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="L7" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="18"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2390,13 +2509,13 @@
       <c r="F8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>392</v>
       </c>
       <c r="H8" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="10" t="b">
+      <c r="I8" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J8" s="5" t="b">
@@ -2405,19 +2524,30 @@
       <c r="K8" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="L8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="O8" s="6"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="L8" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" s="18">
+        <v>3698</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0.88696592752839376</v>
+      </c>
+      <c r="O8" s="16">
+        <v>3.2720389399675504E-2</v>
+      </c>
+      <c r="P8" s="16">
+        <v>8.0313683071930778E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -2435,7 +2565,7 @@
       <c r="H9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I9" s="10" t="b">
+      <c r="I9" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J9" s="5" t="b">
@@ -2447,16 +2577,27 @@
       <c r="L9" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="O9" s="6"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M9" s="18">
+        <v>1184</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0.72635135135135132</v>
+      </c>
+      <c r="O9" s="16">
+        <v>0.10388513513513513</v>
+      </c>
+      <c r="P9" s="16">
+        <v>0.16976351351351351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>238</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -2474,7 +2615,7 @@
       <c r="H10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="10" t="b">
+      <c r="I10" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="b">
@@ -2486,16 +2627,27 @@
       <c r="L10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M10" s="18">
+        <v>1978</v>
+      </c>
+      <c r="N10" s="16">
+        <v>0.77401415571284116</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0.12082912032355915</v>
+      </c>
+      <c r="P10" s="16">
+        <v>0.1051567239635996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -2513,7 +2665,7 @@
       <c r="H11" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="10" t="b">
+      <c r="I11" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J11" s="5" t="b">
@@ -2525,18 +2677,30 @@
       <c r="L11" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M11" s="18">
+        <v>1305</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0.77854406130268194</v>
+      </c>
+      <c r="O11" s="16">
+        <v>0.11264367816091954</v>
+      </c>
+      <c r="P11" s="16">
+        <v>0.10881226053639846</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>205</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -2551,7 +2715,7 @@
       <c r="H12" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="10" t="b">
+      <c r="I12" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="5" t="b">
@@ -2563,15 +2727,27 @@
       <c r="L12" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M12" s="18">
+        <v>2366</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0.79078613693998312</v>
+      </c>
+      <c r="O12" s="16">
+        <v>0.1242603550295858</v>
+      </c>
+      <c r="P12" s="16">
+        <v>8.4953508030431113E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>435</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>88</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2583,13 +2759,13 @@
       <c r="F13" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>400</v>
       </c>
       <c r="H13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="10" t="b">
+      <c r="I13" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J13" s="5" t="b">
@@ -2601,15 +2777,19 @@
       <c r="L13" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M13" s="18"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -2627,7 +2807,7 @@
       <c r="H14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="10" t="b">
+      <c r="I14" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J14" s="5" t="b">
@@ -2639,15 +2819,27 @@
       <c r="L14" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M14" s="18">
+        <v>3450</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0.73217391304347823</v>
+      </c>
+      <c r="O14" s="16">
+        <v>0.14840579710144927</v>
+      </c>
+      <c r="P14" s="16">
+        <v>0.11942028985507247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2665,7 +2857,7 @@
       <c r="H15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="10" t="b">
+      <c r="I15" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J15" s="5" t="b">
@@ -2677,15 +2869,27 @@
       <c r="L15" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M15" s="18">
+        <v>1823</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.7153044432254525</v>
+      </c>
+      <c r="O15" s="16">
+        <v>0.17827756445419637</v>
+      </c>
+      <c r="P15" s="16">
+        <v>0.10641799232035107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
@@ -2703,7 +2907,7 @@
       <c r="H16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="10" t="b">
+      <c r="I16" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J16" s="5" t="b">
@@ -2715,15 +2919,27 @@
       <c r="L16" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M16" s="18">
+        <v>1555</v>
+      </c>
+      <c r="N16" s="16">
+        <v>0.67266881028938907</v>
+      </c>
+      <c r="O16" s="16">
+        <v>0.11639871382636656</v>
+      </c>
+      <c r="P16" s="16">
+        <v>0.21093247588424438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>190</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -2741,7 +2957,7 @@
       <c r="H17" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="10" t="b">
+      <c r="I17" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J17" s="5" t="b">
@@ -2753,15 +2969,27 @@
       <c r="L17" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M17" s="18">
+        <v>1724</v>
+      </c>
+      <c r="N17" s="16">
+        <v>0.62993039443155452</v>
+      </c>
+      <c r="O17" s="16">
+        <v>0.2140371229698376</v>
+      </c>
+      <c r="P17" s="16">
+        <v>0.15603248259860789</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>76</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -2779,7 +3007,7 @@
       <c r="H18" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="10" t="b">
+      <c r="I18" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J18" s="5" t="b">
@@ -2791,15 +3019,27 @@
       <c r="L18" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M18" s="18">
+        <v>3197</v>
+      </c>
+      <c r="N18" s="16">
+        <v>0.79105411323115415</v>
+      </c>
+      <c r="O18" s="16">
+        <v>6.0369096027525805E-2</v>
+      </c>
+      <c r="P18" s="16">
+        <v>0.14857679074131999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>229</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -2811,13 +3051,13 @@
       <c r="F19" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>399</v>
       </c>
       <c r="H19" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="10" t="b">
+      <c r="I19" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J19" s="5" t="b">
@@ -2829,15 +3069,19 @@
       <c r="L19" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M19" s="18"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>229</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -2855,7 +3099,7 @@
       <c r="H20" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I20" s="10" t="b">
+      <c r="I20" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J20" s="5" t="b">
@@ -2867,15 +3111,27 @@
       <c r="L20" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M20" s="18">
+        <v>2125</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.64988235294117647</v>
+      </c>
+      <c r="O20" s="16">
+        <v>0.14023529411764707</v>
+      </c>
+      <c r="P20" s="16">
+        <v>0.20988235294117646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -2893,7 +3149,7 @@
       <c r="H21" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="10" t="b">
+      <c r="I21" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="b">
@@ -2905,15 +3161,27 @@
       <c r="L21" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M21" s="18">
+        <v>1662</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.75932611311672682</v>
+      </c>
+      <c r="O21" s="16">
+        <v>0.15944645006016847</v>
+      </c>
+      <c r="P21" s="16">
+        <v>8.1227436823104696E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>270</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -2931,7 +3199,7 @@
       <c r="H22" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="10" t="b">
+      <c r="I22" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J22" s="5" t="b">
@@ -2943,15 +3211,27 @@
       <c r="L22" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M22" s="18">
+        <v>1936</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0.92407024793388437</v>
+      </c>
+      <c r="O22" s="16">
+        <v>4.5454545454545456E-2</v>
+      </c>
+      <c r="P22" s="16">
+        <v>3.0475206611570247E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>173</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -2969,7 +3249,7 @@
       <c r="H23" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="10" t="b">
+      <c r="I23" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J23" s="5" t="b">
@@ -2981,15 +3261,27 @@
       <c r="L23" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M23" s="18">
+        <v>3605</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0.72704576976421642</v>
+      </c>
+      <c r="O23" s="16">
+        <v>0.18335644937586684</v>
+      </c>
+      <c r="P23" s="16">
+        <v>8.9597780859916779E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>173</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -2998,16 +3290,16 @@
       <c r="E24" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="6" t="s">
         <v>402</v>
       </c>
       <c r="H24" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="10" t="b">
+      <c r="I24" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J24" s="5" t="b">
@@ -3019,15 +3311,19 @@
       <c r="L24" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M24" s="18"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>84</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -3045,7 +3341,7 @@
       <c r="H25" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="10" t="b">
+      <c r="I25" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="b">
@@ -3057,15 +3353,27 @@
       <c r="L25" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M25" s="18">
+        <v>2131</v>
+      </c>
+      <c r="N25" s="16">
+        <v>0.78836227123416236</v>
+      </c>
+      <c r="O25" s="16">
+        <v>0.1365556076959174</v>
+      </c>
+      <c r="P25" s="16">
+        <v>7.5082121069920224E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>223</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -3083,7 +3391,7 @@
       <c r="H26" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="10" t="b">
+      <c r="I26" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="b">
@@ -3095,15 +3403,27 @@
       <c r="L26" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M26" s="18">
+        <v>2944</v>
+      </c>
+      <c r="N26" s="16">
+        <v>0.76358695652173914</v>
+      </c>
+      <c r="O26" s="16">
+        <v>0.16757246376811594</v>
+      </c>
+      <c r="P26" s="16">
+        <v>6.8840579710144928E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>223</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -3121,7 +3441,7 @@
       <c r="H27" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="10" t="b">
+      <c r="I27" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="b">
@@ -3133,15 +3453,27 @@
       <c r="L27" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M27" s="18">
+        <v>1472</v>
+      </c>
+      <c r="N27" s="16">
+        <v>0.76358695652173914</v>
+      </c>
+      <c r="O27" s="16">
+        <v>0.16757246376811594</v>
+      </c>
+      <c r="P27" s="16">
+        <v>6.8840579710144928E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -3159,7 +3491,7 @@
       <c r="H28" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="10" t="b">
+      <c r="I28" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J28" s="5" t="b">
@@ -3171,15 +3503,27 @@
       <c r="L28" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M28" s="18">
+        <v>1764</v>
+      </c>
+      <c r="N28" s="16">
+        <v>0.78401360544217691</v>
+      </c>
+      <c r="O28" s="16">
+        <v>8.5034013605442174E-2</v>
+      </c>
+      <c r="P28" s="16">
+        <v>0.13095238095238096</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -3197,7 +3541,7 @@
       <c r="H29" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="10" t="b">
+      <c r="I29" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J29" s="5" t="b">
@@ -3209,15 +3553,27 @@
       <c r="L29" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M29" s="18">
+        <v>873</v>
+      </c>
+      <c r="N29" s="16">
+        <v>0.80641466208476509</v>
+      </c>
+      <c r="O29" s="16">
+        <v>5.2691867124856816E-2</v>
+      </c>
+      <c r="P29" s="16">
+        <v>0.14089347079037801</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="3" t="s">
@@ -3235,7 +3591,7 @@
       <c r="H30" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="10" t="b">
+      <c r="I30" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J30" s="5" t="b">
@@ -3247,15 +3603,27 @@
       <c r="L30" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M30" s="18">
+        <v>1971</v>
+      </c>
+      <c r="N30" s="16">
+        <v>0.63774733637747349</v>
+      </c>
+      <c r="O30" s="16">
+        <v>0.15677321156773211</v>
+      </c>
+      <c r="P30" s="16">
+        <v>0.20547945205479451</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -3273,7 +3641,7 @@
       <c r="H31" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="10" t="b">
+      <c r="I31" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J31" s="5" t="b">
@@ -3285,15 +3653,27 @@
       <c r="L31" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M31" s="18">
+        <v>3037</v>
+      </c>
+      <c r="N31" s="16">
+        <v>0.90286466908133023</v>
+      </c>
+      <c r="O31" s="16">
+        <v>5.6634837010207439E-2</v>
+      </c>
+      <c r="P31" s="16">
+        <v>4.0500493908462297E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>419</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>194</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -3311,7 +3691,7 @@
       <c r="H32" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I32" s="10" t="b">
+      <c r="I32" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J32" s="5" t="b">
@@ -3323,18 +3703,30 @@
       <c r="L32" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M32" s="18">
+        <v>1067</v>
+      </c>
+      <c r="N32" s="16">
+        <v>0.59418931583880041</v>
+      </c>
+      <c r="O32" s="16">
+        <v>0.25773195876288657</v>
+      </c>
+      <c r="P32" s="16">
+        <v>0.14807872539831302</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>126</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -3349,7 +3741,7 @@
       <c r="H33" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="10" t="b">
+      <c r="I33" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J33" s="5" t="b">
@@ -3361,15 +3753,27 @@
       <c r="L33" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M33" s="18">
+        <v>4119</v>
+      </c>
+      <c r="N33" s="16">
+        <v>0.85166302500606939</v>
+      </c>
+      <c r="O33" s="16">
+        <v>0.10900704054382132</v>
+      </c>
+      <c r="P33" s="16">
+        <v>3.9329934450109252E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -3387,7 +3791,7 @@
       <c r="H34" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="10" t="b">
+      <c r="I34" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J34" s="5" t="b">
@@ -3396,24 +3800,28 @@
       <c r="K34" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="L34" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="L34" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M34" s="18"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>273</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>388</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -3425,7 +3833,7 @@
       <c r="H35" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="10" t="b">
+      <c r="I35" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J35" s="5" t="b">
@@ -3437,15 +3845,27 @@
       <c r="L35" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M35" s="18">
+        <v>1742</v>
+      </c>
+      <c r="N35" s="16">
+        <v>0.78243398392652119</v>
+      </c>
+      <c r="O35" s="16">
+        <v>0.13260619977037888</v>
+      </c>
+      <c r="P35" s="16">
+        <v>8.4959816303099886E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -3463,7 +3883,7 @@
       <c r="H36" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="10" t="b">
+      <c r="I36" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J36" s="5" t="b">
@@ -3475,15 +3895,27 @@
       <c r="L36" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M36" s="18">
+        <v>5130</v>
+      </c>
+      <c r="N36" s="16">
+        <v>0.8267056530214425</v>
+      </c>
+      <c r="O36" s="16">
+        <v>7.2904483430799222E-2</v>
+      </c>
+      <c r="P36" s="16">
+        <v>0.10038986354775828</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -3495,13 +3927,13 @@
       <c r="F37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="6" t="s">
         <v>397</v>
       </c>
       <c r="H37" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="10" t="b">
+      <c r="I37" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J37" s="5" t="b">
@@ -3513,15 +3945,19 @@
       <c r="L37" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M37" s="18"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -3539,7 +3975,7 @@
       <c r="H38" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I38" s="10" t="b">
+      <c r="I38" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J38" s="5" t="b">
@@ -3551,15 +3987,27 @@
       <c r="L38" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M38" s="18">
+        <v>4643</v>
+      </c>
+      <c r="N38" s="16">
+        <v>0.67973293129442169</v>
+      </c>
+      <c r="O38" s="16">
+        <v>0.12448847727762223</v>
+      </c>
+      <c r="P38" s="16">
+        <v>0.19577859142795606</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>102</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -3577,7 +4025,7 @@
       <c r="H39" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="10" t="b">
+      <c r="I39" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J39" s="5" t="b">
@@ -3589,15 +4037,27 @@
       <c r="L39" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M39" s="18">
+        <v>3456</v>
+      </c>
+      <c r="N39" s="16">
+        <v>0.72309027777777779</v>
+      </c>
+      <c r="O39" s="16">
+        <v>0.12210648148148148</v>
+      </c>
+      <c r="P39" s="16">
+        <v>0.15480324074074073</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>212</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -3615,7 +4075,7 @@
       <c r="H40" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="10" t="b">
+      <c r="I40" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J40" s="5" t="b">
@@ -3627,15 +4087,27 @@
       <c r="L40" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M40" s="18">
+        <v>1235</v>
+      </c>
+      <c r="N40" s="16">
+        <v>0.63967611336032393</v>
+      </c>
+      <c r="O40" s="16">
+        <v>0.24453441295546557</v>
+      </c>
+      <c r="P40" s="16">
+        <v>0.11578947368421053</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D41" s="3" t="s">
@@ -3644,7 +4116,7 @@
       <c r="E41" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="7" t="s">
         <v>385</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -3653,7 +4125,7 @@
       <c r="H41" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="10" t="b">
+      <c r="I41" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J41" s="5" t="b">
@@ -3665,15 +4137,27 @@
       <c r="L41" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M41" s="18">
+        <v>1143</v>
+      </c>
+      <c r="N41" s="16">
+        <v>0.84864391951006124</v>
+      </c>
+      <c r="O41" s="16">
+        <v>6.8241469816272965E-2</v>
+      </c>
+      <c r="P41" s="16">
+        <v>8.3114610673665795E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>458</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D42" s="3" t="s">
@@ -3691,7 +4175,7 @@
       <c r="H42" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I42" s="10" t="b">
+      <c r="I42" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J42" s="5" t="b">
@@ -3703,15 +4187,27 @@
       <c r="L42" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M42" s="18">
+        <v>2908</v>
+      </c>
+      <c r="N42" s="16">
+        <v>0.78129298486932597</v>
+      </c>
+      <c r="O42" s="16">
+        <v>0.11004126547455295</v>
+      </c>
+      <c r="P42" s="16">
+        <v>0.10866574965612105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>129</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -3729,7 +4225,7 @@
       <c r="H43" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="10" t="b">
+      <c r="I43" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J43" s="5" t="b">
@@ -3741,15 +4237,27 @@
       <c r="L43" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M43" s="18">
+        <v>5130</v>
+      </c>
+      <c r="N43" s="16">
+        <v>0.8267056530214425</v>
+      </c>
+      <c r="O43" s="16">
+        <v>7.2904483430799222E-2</v>
+      </c>
+      <c r="P43" s="16">
+        <v>0.10038986354775828</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>142</v>
       </c>
       <c r="D44" s="3" t="s">
@@ -3767,7 +4275,7 @@
       <c r="H44" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I44" s="10" t="b">
+      <c r="I44" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J44" s="5" t="b">
@@ -3779,15 +4287,27 @@
       <c r="L44" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M44" s="18">
+        <v>1185</v>
+      </c>
+      <c r="N44" s="16">
+        <v>0.69620253164556967</v>
+      </c>
+      <c r="O44" s="16">
+        <v>0.16708860759493671</v>
+      </c>
+      <c r="P44" s="16">
+        <v>0.13670886075949368</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -3805,7 +4325,7 @@
       <c r="H45" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I45" s="10" t="b">
+      <c r="I45" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J45" s="5" t="b">
@@ -3817,15 +4337,27 @@
       <c r="L45" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M45" s="18">
+        <v>2996</v>
+      </c>
+      <c r="N45" s="16">
+        <v>0.69559412550066757</v>
+      </c>
+      <c r="O45" s="16">
+        <v>0.16555407209612816</v>
+      </c>
+      <c r="P45" s="16">
+        <v>0.13885180240320427</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
@@ -3843,7 +4375,7 @@
       <c r="H46" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="10" t="b">
+      <c r="I46" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J46" s="5" t="b">
@@ -3855,18 +4387,30 @@
       <c r="L46" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M46" s="18">
+        <v>2539</v>
+      </c>
+      <c r="N46" s="16">
+        <v>0.80661677825915712</v>
+      </c>
+      <c r="O46" s="16">
+        <v>0.12012603387160299</v>
+      </c>
+      <c r="P46" s="16">
+        <v>7.3257187869239862E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>254</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -3881,7 +4425,7 @@
       <c r="H47" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I47" s="10" t="b">
+      <c r="I47" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J47" s="5" t="b">
@@ -3893,21 +4437,33 @@
       <c r="L47" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M47" s="18">
+        <v>2097</v>
+      </c>
+      <c r="N47" s="16">
+        <v>0.66046733428707682</v>
+      </c>
+      <c r="O47" s="16">
+        <v>0.10348116356700048</v>
+      </c>
+      <c r="P47" s="16">
+        <v>0.23605150214592274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>279</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="6" t="s">
         <v>386</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -3919,7 +4475,7 @@
       <c r="H48" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I48" s="10" t="b">
+      <c r="I48" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J48" s="5" t="b">
@@ -3931,18 +4487,30 @@
       <c r="L48" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M48" s="18">
+        <v>3189</v>
+      </c>
+      <c r="N48" s="16">
+        <v>0.66509877704609599</v>
+      </c>
+      <c r="O48" s="16">
+        <v>0.11571025399811853</v>
+      </c>
+      <c r="P48" s="16">
+        <v>0.21919096895578552</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>133</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -3957,7 +4525,7 @@
       <c r="H49" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="10" t="b">
+      <c r="I49" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J49" s="5" t="b">
@@ -3969,15 +4537,27 @@
       <c r="L49" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M49" s="18">
+        <v>4793</v>
+      </c>
+      <c r="N49" s="16">
+        <v>0.77842687252242848</v>
+      </c>
+      <c r="O49" s="16">
+        <v>9.4721468808679321E-2</v>
+      </c>
+      <c r="P49" s="16">
+        <v>0.12685165866889214</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>186</v>
       </c>
       <c r="D50" s="3" t="s">
@@ -3995,7 +4575,7 @@
       <c r="H50" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I50" s="10" t="b">
+      <c r="I50" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J50" s="5" t="b">
@@ -4007,15 +4587,27 @@
       <c r="L50" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M50" s="18">
+        <v>1222</v>
+      </c>
+      <c r="N50" s="16">
+        <v>0.67021276595744683</v>
+      </c>
+      <c r="O50" s="16">
+        <v>0.13011456628477905</v>
+      </c>
+      <c r="P50" s="16">
+        <v>0.19967266775777415</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>118</v>
       </c>
       <c r="D51" s="3" t="s">
@@ -4033,7 +4625,7 @@
       <c r="H51" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="10" t="b">
+      <c r="I51" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J51" s="5" t="b">
@@ -4045,15 +4637,27 @@
       <c r="L51" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M51" s="18">
+        <v>2729.6</v>
+      </c>
+      <c r="N51" s="16">
+        <v>0.73036342321219228</v>
+      </c>
+      <c r="O51" s="16">
+        <v>0.11400937866354044</v>
+      </c>
+      <c r="P51" s="16">
+        <v>0.15562719812426731</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>118</v>
       </c>
       <c r="D52" s="3" t="s">
@@ -4071,7 +4675,7 @@
       <c r="H52" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I52" s="10" t="b">
+      <c r="I52" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J52" s="5" t="b">
@@ -4083,15 +4687,27 @@
       <c r="L52" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M52" s="18">
+        <v>682.4</v>
+      </c>
+      <c r="N52" s="16">
+        <v>0.73036342321219228</v>
+      </c>
+      <c r="O52" s="16">
+        <v>0.11400937866354044</v>
+      </c>
+      <c r="P52" s="16">
+        <v>0.15562719812426731</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>286</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -4109,7 +4725,7 @@
       <c r="H53" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I53" s="10" t="b">
+      <c r="I53" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J53" s="5" t="b">
@@ -4121,15 +4737,27 @@
       <c r="L53" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M53" s="18">
+        <v>3929</v>
+      </c>
+      <c r="N53" s="16">
+        <v>0.78849580045813172</v>
+      </c>
+      <c r="O53" s="16">
+        <v>0.11300585390684653</v>
+      </c>
+      <c r="P53" s="16">
+        <v>9.8498345635021634E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>286</v>
       </c>
       <c r="D54" s="3" t="s">
@@ -4147,7 +4775,7 @@
       <c r="H54" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="10" t="b">
+      <c r="I54" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J54" s="5" t="b">
@@ -4159,15 +4787,27 @@
       <c r="L54" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M54" s="18">
+        <v>3559</v>
+      </c>
+      <c r="N54" s="16">
+        <v>0.83675189660016858</v>
+      </c>
+      <c r="O54" s="16">
+        <v>5.4790671536948582E-2</v>
+      </c>
+      <c r="P54" s="16">
+        <v>0.10845743186288283</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="12" t="s">
         <v>467</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="9" t="s">
         <v>72</v>
       </c>
       <c r="D55" s="3" t="s">
@@ -4185,7 +4825,7 @@
       <c r="H55" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I55" s="10" t="b">
+      <c r="I55" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J55" s="5" t="b">
@@ -4197,15 +4837,27 @@
       <c r="L55" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M55" s="18">
+        <v>786</v>
+      </c>
+      <c r="N55" s="16">
+        <v>0.70356234096692116</v>
+      </c>
+      <c r="O55" s="16">
+        <v>0.17302798982188294</v>
+      </c>
+      <c r="P55" s="16">
+        <v>0.12340966921119594</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>293</v>
       </c>
       <c r="D56" s="3" t="s">
@@ -4223,7 +4875,7 @@
       <c r="H56" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I56" s="10" t="b">
+      <c r="I56" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J56" s="5" t="b">
@@ -4235,15 +4887,27 @@
       <c r="L56" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M56" s="18">
+        <v>3450</v>
+      </c>
+      <c r="N56" s="16">
+        <v>0.73217391304347823</v>
+      </c>
+      <c r="O56" s="16">
+        <v>0.14840579710144927</v>
+      </c>
+      <c r="P56" s="16">
+        <v>0.11942028985507247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>146</v>
       </c>
       <c r="D57" s="3" t="s">
@@ -4261,7 +4925,7 @@
       <c r="H57" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I57" s="10" t="b">
+      <c r="I57" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J57" s="5" t="b">
@@ -4273,15 +4937,27 @@
       <c r="L57" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M57" s="18">
+        <v>2908</v>
+      </c>
+      <c r="N57" s="16">
+        <v>0.74381017881705636</v>
+      </c>
+      <c r="O57" s="16">
+        <v>0.15061898211829436</v>
+      </c>
+      <c r="P57" s="16">
+        <v>0.10557083906464924</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="3" t="s">
@@ -4290,7 +4966,7 @@
       <c r="E58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="13" t="s">
         <v>8</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -4299,7 +4975,7 @@
       <c r="H58" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I58" s="10" t="b">
+      <c r="I58" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J58" s="5" t="b">
@@ -4311,15 +4987,27 @@
       <c r="L58" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M58" s="18">
+        <v>3096</v>
+      </c>
+      <c r="N58" s="16">
+        <v>0.71447028423772607</v>
+      </c>
+      <c r="O58" s="16">
+        <v>0.16957364341085271</v>
+      </c>
+      <c r="P58" s="16">
+        <v>0.11595607235142119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>152</v>
       </c>
       <c r="D59" s="3" t="s">
@@ -4337,7 +5025,7 @@
       <c r="H59" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I59" s="10" t="b">
+      <c r="I59" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J59" s="5" t="b">
@@ -4349,15 +5037,27 @@
       <c r="L59" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M59" s="18">
+        <v>1708</v>
+      </c>
+      <c r="N59" s="16">
+        <v>0.63056206088992972</v>
+      </c>
+      <c r="O59" s="16">
+        <v>0.13466042154566746</v>
+      </c>
+      <c r="P59" s="16">
+        <v>0.23477751756440282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="12" t="s">
         <v>415</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="3" t="s">
@@ -4375,7 +5075,7 @@
       <c r="H60" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I60" s="10" t="b">
+      <c r="I60" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J60" s="5" t="b">
@@ -4387,15 +5087,27 @@
       <c r="L60" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M60" s="18">
+        <v>1372</v>
+      </c>
+      <c r="N60" s="16">
+        <v>0.70189504373177847</v>
+      </c>
+      <c r="O60" s="16">
+        <v>0.17055393586005832</v>
+      </c>
+      <c r="P60" s="16">
+        <v>0.12755102040816327</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>156</v>
       </c>
       <c r="D61" s="3" t="s">
@@ -4413,7 +5125,7 @@
       <c r="H61" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I61" s="10" t="b">
+      <c r="I61" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J61" s="5" t="b">
@@ -4425,15 +5137,27 @@
       <c r="L61" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M61" s="18">
+        <v>776</v>
+      </c>
+      <c r="N61" s="16">
+        <v>0.759020618556701</v>
+      </c>
+      <c r="O61" s="16">
+        <v>0.11211340206185567</v>
+      </c>
+      <c r="P61" s="16">
+        <v>0.12886597938144329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D62" s="3" t="s">
@@ -4451,7 +5175,7 @@
       <c r="H62" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I62" s="10" t="b">
+      <c r="I62" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J62" s="5" t="b">
@@ -4463,15 +5187,27 @@
       <c r="L62" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M62" s="18">
+        <v>1327</v>
+      </c>
+      <c r="N62" s="16">
+        <v>0.75131876412961573</v>
+      </c>
+      <c r="O62" s="16">
+        <v>0.13187641296156744</v>
+      </c>
+      <c r="P62" s="16">
+        <v>0.11680482290881689</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D63" s="3" t="s">
@@ -4483,13 +5219,13 @@
       <c r="F63" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="G63" s="6" t="s">
         <v>393</v>
       </c>
       <c r="H63" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I63" s="10" t="b">
+      <c r="I63" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J63" s="5" t="b">
@@ -4501,15 +5237,19 @@
       <c r="L63" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M63" s="18"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -4527,7 +5267,7 @@
       <c r="H64" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I64" s="10" t="b">
+      <c r="I64" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J64" s="5" t="b">
@@ -4539,15 +5279,27 @@
       <c r="L64" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M64" s="18">
+        <v>3840</v>
+      </c>
+      <c r="N64" s="16">
+        <v>0.75390625</v>
+      </c>
+      <c r="O64" s="16">
+        <v>0.12005208333333334</v>
+      </c>
+      <c r="P64" s="16">
+        <v>0.12604166666666666</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -4559,13 +5311,13 @@
       <c r="F65" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="G65" s="6" t="s">
         <v>395</v>
       </c>
       <c r="H65" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I65" s="10" t="b">
+      <c r="I65" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J65" s="5" t="b">
@@ -4577,15 +5329,19 @@
       <c r="L65" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M65" s="18"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>64</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>163</v>
       </c>
       <c r="D66" s="3" t="s">
@@ -4603,7 +5359,7 @@
       <c r="H66" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I66" s="10" t="b">
+      <c r="I66" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J66" s="5" t="b">
@@ -4615,15 +5371,27 @@
       <c r="L66" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M66" s="18">
+        <v>939</v>
+      </c>
+      <c r="N66" s="16">
+        <v>0.74334398296059634</v>
+      </c>
+      <c r="O66" s="16">
+        <v>0.16080937167199147</v>
+      </c>
+      <c r="P66" s="16">
+        <v>9.5846645367412137E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>65</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>167</v>
       </c>
       <c r="D67" s="3" t="s">
@@ -4635,13 +5403,13 @@
       <c r="F67" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="G67" s="7" t="s">
+      <c r="G67" s="6" t="s">
         <v>398</v>
       </c>
       <c r="H67" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I67" s="10" t="b">
+      <c r="I67" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J67" s="5" t="b">
@@ -4653,15 +5421,19 @@
       <c r="L67" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M67" s="18"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>66</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="9" t="s">
         <v>167</v>
       </c>
       <c r="D68" s="3" t="s">
@@ -4679,7 +5451,7 @@
       <c r="H68" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I68" s="10" t="b">
+      <c r="I68" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J68" s="5" t="b">
@@ -4691,15 +5463,27 @@
       <c r="L68" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M68" s="18">
+        <v>4320</v>
+      </c>
+      <c r="N68" s="16">
+        <v>0.77361111111111114</v>
+      </c>
+      <c r="O68" s="16">
+        <v>0.11435185185185186</v>
+      </c>
+      <c r="P68" s="16">
+        <v>0.11203703703703703</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>67</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="9" t="s">
         <v>177</v>
       </c>
       <c r="D69" s="3" t="s">
@@ -4717,7 +5501,7 @@
       <c r="H69" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I69" s="10" t="b">
+      <c r="I69" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J69" s="5" t="b">
@@ -4729,15 +5513,27 @@
       <c r="L69" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M69" s="18">
+        <v>737</v>
+      </c>
+      <c r="N69" s="16">
+        <v>0.78018995929443702</v>
+      </c>
+      <c r="O69" s="16">
+        <v>0.12347354138398914</v>
+      </c>
+      <c r="P69" s="16">
+        <v>9.6336499321573954E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>68</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="9" t="s">
         <v>208</v>
       </c>
       <c r="D70" s="3" t="s">
@@ -4755,7 +5551,7 @@
       <c r="H70" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I70" s="10" t="b">
+      <c r="I70" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J70" s="5" t="b">
@@ -4767,15 +5563,27 @@
       <c r="L70" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M70" s="18">
+        <v>939</v>
+      </c>
+      <c r="N70" s="16">
+        <v>0.6911608093716719</v>
+      </c>
+      <c r="O70" s="16">
+        <v>0.13844515441959532</v>
+      </c>
+      <c r="P70" s="16">
+        <v>0.1703940362087327</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>69</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="9" t="s">
         <v>198</v>
       </c>
       <c r="D71" s="3" t="s">
@@ -4793,7 +5601,7 @@
       <c r="H71" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I71" s="10" t="b">
+      <c r="I71" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J71" s="5" t="b">
@@ -4805,15 +5613,27 @@
       <c r="L71" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M71" s="18">
+        <v>2316</v>
+      </c>
+      <c r="N71" s="16">
+        <v>0.66018998272884288</v>
+      </c>
+      <c r="O71" s="16">
+        <v>0.2189119170984456</v>
+      </c>
+      <c r="P71" s="16">
+        <v>0.12089810017271158</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>70</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="9" t="s">
         <v>198</v>
       </c>
       <c r="D72" s="3" t="s">
@@ -4825,13 +5645,13 @@
       <c r="F72" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="G72" s="7" t="s">
+      <c r="G72" s="6" t="s">
         <v>394</v>
       </c>
       <c r="H72" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I72" s="10" t="b">
+      <c r="I72" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J72" s="5" t="b">
@@ -4843,15 +5663,19 @@
       <c r="L72" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M72" s="18"/>
+      <c r="N72" s="16"/>
+      <c r="O72" s="16"/>
+      <c r="P72" s="16"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>71</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="9" t="s">
         <v>256</v>
       </c>
       <c r="D73" s="3" t="s">
@@ -4863,13 +5687,13 @@
       <c r="F73" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="G73" s="7" t="s">
+      <c r="G73" s="6" t="s">
         <v>396</v>
       </c>
       <c r="H73" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I73" s="10" t="b">
+      <c r="I73" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J73" s="5" t="b">
@@ -4881,15 +5705,19 @@
       <c r="L73" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M73" s="18"/>
+      <c r="N73" s="16"/>
+      <c r="O73" s="16"/>
+      <c r="P73" s="16"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>72</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B74" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="9" t="s">
         <v>256</v>
       </c>
       <c r="D74" s="3" t="s">
@@ -4901,13 +5729,13 @@
       <c r="F74" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="G74" s="7" t="s">
+      <c r="G74" s="6" t="s">
         <v>403</v>
       </c>
       <c r="H74" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I74" s="10" t="b">
+      <c r="I74" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J74" s="5" t="b">
@@ -4919,15 +5747,19 @@
       <c r="L74" s="5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M74" s="18"/>
+      <c r="N74" s="16"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="16"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>73</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="9" t="s">
         <v>256</v>
       </c>
       <c r="D75" s="3" t="s">
@@ -4945,7 +5777,7 @@
       <c r="H75" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I75" s="10" t="b">
+      <c r="I75" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J75" s="5" t="b">
@@ -4957,15 +5789,27 @@
       <c r="L75" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M75" s="18">
+        <v>1212</v>
+      </c>
+      <c r="N75" s="16">
+        <v>0.75165016501650161</v>
+      </c>
+      <c r="O75" s="16">
+        <v>0.1476897689768977</v>
+      </c>
+      <c r="P75" s="16">
+        <v>0.10066006600660066</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>74</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="9" t="s">
         <v>291</v>
       </c>
       <c r="D76" s="3" t="s">
@@ -4983,7 +5827,7 @@
       <c r="H76" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I76" s="10" t="b">
+      <c r="I76" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J76" s="5" t="b">
@@ -4995,15 +5839,27 @@
       <c r="L76" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M76" s="18">
+        <v>2032</v>
+      </c>
+      <c r="N76" s="16">
+        <v>0.7514763779527559</v>
+      </c>
+      <c r="O76" s="16">
+        <v>0.11515748031496063</v>
+      </c>
+      <c r="P76" s="16">
+        <v>0.13336614173228348</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>75</v>
       </c>
-      <c r="B77" s="13" t="s">
+      <c r="B77" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="9" t="s">
         <v>217</v>
       </c>
       <c r="D77" s="3" t="s">
@@ -5021,7 +5877,7 @@
       <c r="H77" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I77" s="10" t="b">
+      <c r="I77" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J77" s="5" t="b">
@@ -5030,18 +5886,22 @@
       <c r="K77" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="L77" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="L77" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M77" s="18"/>
+      <c r="N77" s="16"/>
+      <c r="O77" s="16"/>
+      <c r="P77" s="16"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>76</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="9" t="s">
         <v>217</v>
       </c>
       <c r="D78" s="3" t="s">
@@ -5053,13 +5913,13 @@
       <c r="F78" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G78" s="7" t="s">
+      <c r="G78" s="6" t="s">
         <v>404</v>
       </c>
       <c r="H78" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I78" s="10" t="b">
+      <c r="I78" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J78" s="5" t="b">
@@ -5068,18 +5928,30 @@
       <c r="K78" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="L78" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="L78" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M78" s="18">
+        <v>2884</v>
+      </c>
+      <c r="N78" s="16">
+        <v>0.76248266296809986</v>
+      </c>
+      <c r="O78" s="16">
+        <v>0.17649098474341193</v>
+      </c>
+      <c r="P78" s="16">
+        <v>6.1026352288488211E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>77</v>
       </c>
-      <c r="B79" s="13" t="s">
+      <c r="B79" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C79" s="9" t="s">
         <v>219</v>
       </c>
       <c r="D79" s="3" t="s">
@@ -5097,7 +5969,7 @@
       <c r="H79" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I79" s="10" t="b">
+      <c r="I79" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J79" s="5" t="b">
@@ -5109,15 +5981,27 @@
       <c r="L79" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M79" s="18">
+        <v>1467</v>
+      </c>
+      <c r="N79" s="16">
+        <v>0.74778459441036127</v>
+      </c>
+      <c r="O79" s="16">
+        <v>0.1492842535787321</v>
+      </c>
+      <c r="P79" s="16">
+        <v>0.10293115201090661</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>78</v>
       </c>
-      <c r="B80" s="13" t="s">
+      <c r="B80" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="C80" s="10" t="s">
+      <c r="C80" s="9" t="s">
         <v>297</v>
       </c>
       <c r="D80" s="3" t="s">
@@ -5135,7 +6019,7 @@
       <c r="H80" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I80" s="10" t="b">
+      <c r="I80" s="9" t="b">
         <v>1</v>
       </c>
       <c r="J80" s="5" t="b">
@@ -5147,15 +6031,27 @@
       <c r="L80" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M80" s="18">
+        <v>1695</v>
+      </c>
+      <c r="N80" s="16">
+        <v>0.87197640117994102</v>
+      </c>
+      <c r="O80" s="16">
+        <v>6.2536873156342182E-2</v>
+      </c>
+      <c r="P80" s="16">
+        <v>6.5486725663716813E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>79</v>
       </c>
-      <c r="B81" s="13" t="s">
+      <c r="B81" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="C81" s="9" t="s">
         <v>300</v>
       </c>
       <c r="D81" s="3" t="s">
@@ -5173,7 +6069,7 @@
       <c r="H81" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I81" s="10" t="b">
+      <c r="I81" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J81" s="5" t="b">
@@ -5185,15 +6081,27 @@
       <c r="L81" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M81" s="18">
+        <v>988</v>
+      </c>
+      <c r="N81" s="16">
+        <v>0.74898785425101211</v>
+      </c>
+      <c r="O81" s="16">
+        <v>0.11437246963562753</v>
+      </c>
+      <c r="P81" s="16">
+        <v>0.13663967611336034</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>80</v>
       </c>
-      <c r="B82" s="13" t="s">
+      <c r="B82" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="C82" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D82" s="3" t="s">
@@ -5211,7 +6119,7 @@
       <c r="H82" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I82" s="10" t="b">
+      <c r="I82" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J82" s="5" t="b">
@@ -5223,15 +6131,27 @@
       <c r="L82" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M82" s="18">
+        <v>1599</v>
+      </c>
+      <c r="N82" s="16">
+        <v>0.75984990619136961</v>
+      </c>
+      <c r="O82" s="16">
+        <v>0.13195747342088807</v>
+      </c>
+      <c r="P82" s="16">
+        <v>0.10819262038774234</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>81</v>
       </c>
-      <c r="B83" s="13" t="s">
+      <c r="B83" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="9" t="s">
         <v>234</v>
       </c>
       <c r="D83" s="3" t="s">
@@ -5243,13 +6163,13 @@
       <c r="F83" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="G83" s="7" t="s">
+      <c r="G83" s="6" t="s">
         <v>391</v>
       </c>
       <c r="H83" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I83" s="10" t="b">
+      <c r="I83" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J83" s="5" t="b">
@@ -5258,18 +6178,30 @@
       <c r="K83" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="L83" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="L83" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M83" s="18">
+        <v>1361</v>
+      </c>
+      <c r="N83" s="16">
+        <v>0.72446730345334309</v>
+      </c>
+      <c r="O83" s="16">
+        <v>0.1807494489346069</v>
+      </c>
+      <c r="P83" s="16">
+        <v>9.4783247612049967E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>82</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B84" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C84" s="9" t="s">
         <v>242</v>
       </c>
       <c r="D84" s="3" t="s">
@@ -5287,7 +6219,7 @@
       <c r="H84" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I84" s="10" t="b">
+      <c r="I84" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J84" s="5" t="b">
@@ -5299,15 +6231,27 @@
       <c r="L84" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M84" s="18">
+        <v>3037</v>
+      </c>
+      <c r="N84" s="16">
+        <v>0.60059269015475802</v>
+      </c>
+      <c r="O84" s="16">
+        <v>0.112940401712216</v>
+      </c>
+      <c r="P84" s="16">
+        <v>0.286466908133026</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>83</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C85" s="9" t="s">
         <v>246</v>
       </c>
       <c r="D85" s="3" t="s">
@@ -5325,7 +6269,7 @@
       <c r="H85" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I85" s="10" t="b">
+      <c r="I85" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J85" s="5" t="b">
@@ -5337,15 +6281,27 @@
       <c r="L85" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M85" s="18">
+        <v>1378</v>
+      </c>
+      <c r="N85" s="16">
+        <v>0.67489114658925975</v>
+      </c>
+      <c r="O85" s="16">
+        <v>0.1204644412191582</v>
+      </c>
+      <c r="P85" s="16">
+        <v>0.204644412191582</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>84</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B86" s="12" t="s">
         <v>429</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C86" s="9" t="s">
         <v>181</v>
       </c>
       <c r="D86" s="3" t="s">
@@ -5363,7 +6319,7 @@
       <c r="H86" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I86" s="10" t="b">
+      <c r="I86" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J86" s="5" t="b">
@@ -5375,15 +6331,27 @@
       <c r="L86" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M86" s="18">
+        <v>1898</v>
+      </c>
+      <c r="N86" s="16">
+        <v>0.71601685985247621</v>
+      </c>
+      <c r="O86" s="16">
+        <v>3.3192834562697573E-2</v>
+      </c>
+      <c r="P86" s="16">
+        <v>0.25079030558482612</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>85</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C87" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D87" s="3" t="s">
@@ -5401,7 +6369,7 @@
       <c r="H87" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I87" s="10" t="b">
+      <c r="I87" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J87" s="5" t="b">
@@ -5413,15 +6381,27 @@
       <c r="L87" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M87" s="18">
+        <v>4793</v>
+      </c>
+      <c r="N87" s="16">
+        <v>0.77842687252242848</v>
+      </c>
+      <c r="O87" s="16">
+        <v>9.4721468808679321E-2</v>
+      </c>
+      <c r="P87" s="16">
+        <v>0.12685165866889214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>86</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B88" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C88" s="9" t="s">
         <v>250</v>
       </c>
       <c r="D88" s="3" t="s">
@@ -5439,7 +6419,7 @@
       <c r="H88" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="I88" s="10" t="b">
+      <c r="I88" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J88" s="5" t="b">
@@ -5451,15 +6431,27 @@
       <c r="L88" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M88" s="18">
+        <v>671</v>
+      </c>
+      <c r="N88" s="16">
+        <v>0.77794336810730258</v>
+      </c>
+      <c r="O88" s="16">
+        <v>0.20268256333830104</v>
+      </c>
+      <c r="P88" s="16">
+        <v>1.9374068554396422E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>87</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C89" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D89" s="3" t="s">
@@ -5477,7 +6469,7 @@
       <c r="H89" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I89" s="10" t="b">
+      <c r="I89" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J89" s="5" t="b">
@@ -5489,15 +6481,27 @@
       <c r="L89" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="M89" s="18">
+        <v>2751</v>
+      </c>
+      <c r="N89" s="16">
+        <v>0.83133406034169399</v>
+      </c>
+      <c r="O89" s="16">
+        <v>8.8331515812431843E-2</v>
+      </c>
+      <c r="P89" s="16">
+        <v>8.0334423845874234E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>88</v>
       </c>
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C90" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D90" s="3" t="s">
@@ -5509,13 +6513,13 @@
       <c r="F90" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="G90" s="7" t="s">
+      <c r="G90" s="6" t="s">
         <v>401</v>
       </c>
       <c r="H90" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I90" s="10" t="b">
+      <c r="I90" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J90" s="5" t="b">
@@ -5527,6 +6531,31 @@
       <c r="L90" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="M90" s="18"/>
+      <c r="N90" s="16"/>
+      <c r="O90" s="16"/>
+      <c r="P90" s="16"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M91" s="18"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M92" s="18"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M93" s="18"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M94" s="18"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M95" s="18"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M96" s="18"/>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M97" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:L90" xr:uid="{5886180B-99A2-4FA7-8473-800F0FA8BE14}">
@@ -5537,7 +6566,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L90">
     <sortCondition ref="B1"/>
   </sortState>
-  <conditionalFormatting sqref="I2:L90 I1:I1048576">
+  <conditionalFormatting sqref="I1:I1048576 I2:M90">
     <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added new info to hospitals (notes, perc unknown)
</commit_message>
<xml_diff>
--- a/packages/processing/docs/Ziekenhuislocaties.xlsx
+++ b/packages/processing/docs/Ziekenhuislocaties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\home\erik\dev\test_ziekenhuizen\packages\processing\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADAC26B-27E9-40EB-AF4D-BE4F2C3AAB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D729C9-81EE-46A5-ABC0-8C6F822C4258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="506">
   <si>
     <t>plaats</t>
   </si>
@@ -1498,6 +1498,57 @@
   </si>
   <si>
     <t>perc1lLijnThuis</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Molengracht</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Bergen op Zoom</t>
+  </si>
+  <si>
+    <t>Initiele verdeling productie obv SEH bezoeken 2/3</t>
+  </si>
+  <si>
+    <t>Initiele verdeling productie obv SEH bezoeken 1/3</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Zwolle</t>
+  </si>
+  <si>
+    <t>Initiele verdeling productie obv bedden 8/10</t>
+  </si>
+  <si>
+    <t>Initiele verdeling productie obv bedden 2/10</t>
+  </si>
+  <si>
+    <t>Initiele verdeling productie obv suites 4/7</t>
+  </si>
+  <si>
+    <t>Initiele verdeling productie obv suites 3/7</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Utrecht</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Blaricum</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Emmen</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie UMCU</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Harderwijk</t>
+  </si>
+  <si>
+    <t>Initieel alle productie toebedeeld aan locatie Heerlen</t>
+  </si>
+  <si>
+    <t>percOnbekend</t>
+  </si>
+  <si>
+    <t>notitie</t>
   </si>
 </sst>
 </file>
@@ -2122,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P97"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2148,7 +2199,7 @@
     <col min="17" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>483</v>
       </c>
@@ -2197,8 +2248,14 @@
       <c r="P1" s="15" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2239,16 +2296,19 @@
         <v>1608</v>
       </c>
       <c r="N2" s="16">
-        <v>0.79850746268656714</v>
+        <v>0.79166666699999999</v>
       </c>
       <c r="O2" s="16">
-        <v>0.10261194029850747</v>
+        <v>0.10261194</v>
       </c>
       <c r="P2" s="16">
-        <v>9.8880597014925367E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>9.8880597000000001E-2</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>6.8407959999999997E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2289,16 +2349,19 @@
         <v>1764</v>
       </c>
       <c r="N3" s="16">
-        <v>0.68367346938775508</v>
+        <v>0.65759637199999998</v>
       </c>
       <c r="O3" s="16">
-        <v>0.11848072562358276</v>
+        <v>0.11848072599999999</v>
       </c>
       <c r="P3" s="16">
-        <v>0.19784580498866214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.19784580500000001</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2.6077098E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2339,16 +2402,19 @@
         <v>2847</v>
       </c>
       <c r="N4" s="16">
-        <v>0.74745345978222688</v>
+        <v>0.74007727400000001</v>
       </c>
       <c r="O4" s="16">
-        <v>0.12820512820512819</v>
+        <v>0.128205128</v>
       </c>
       <c r="P4" s="16">
-        <v>0.12434141201264488</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.124341412</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>7.3761850000000004E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2389,16 +2455,19 @@
         <v>1852</v>
       </c>
       <c r="N5" s="16">
-        <v>0.63336933045356369</v>
+        <v>0.63174945999999998</v>
       </c>
       <c r="O5" s="16">
-        <v>0.18628509719222464</v>
+        <v>0.18628509700000001</v>
       </c>
       <c r="P5" s="16">
-        <v>0.18034557235421167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.18034557200000001</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1.61987E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2439,16 +2508,19 @@
         <v>1507</v>
       </c>
       <c r="N6" s="16">
-        <v>0.85666887856668883</v>
+        <v>0.85534173899999999</v>
       </c>
       <c r="O6" s="16">
-        <v>6.9011280690112808E-2</v>
+        <v>6.9011280999999994E-2</v>
       </c>
       <c r="P6" s="16">
-        <v>7.4319840743198404E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>7.4319840999999998E-2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1.3271400000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2489,8 +2561,11 @@
       <c r="N7" s="16"/>
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R7" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2531,16 +2606,22 @@
         <v>3698</v>
       </c>
       <c r="N8" s="16">
-        <v>0.88696592752839376</v>
+        <v>0.73823688499999995</v>
       </c>
       <c r="O8" s="16">
-        <v>3.2720389399675504E-2</v>
+        <v>3.2720389000000002E-2</v>
       </c>
       <c r="P8" s="16">
-        <v>8.0313683071930778E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.0313682999999997E-2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.14872904300000001</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2581,16 +2662,19 @@
         <v>1184</v>
       </c>
       <c r="N9" s="16">
-        <v>0.72635135135135132</v>
+        <v>0.72635135100000003</v>
       </c>
       <c r="O9" s="16">
-        <v>0.10388513513513513</v>
+        <v>0.103885135</v>
       </c>
       <c r="P9" s="16">
-        <v>0.16976351351351351</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.169763514</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2631,16 +2715,19 @@
         <v>1978</v>
       </c>
       <c r="N10" s="16">
-        <v>0.77401415571284116</v>
+        <v>0.77249747199999996</v>
       </c>
       <c r="O10" s="16">
-        <v>0.12082912032355915</v>
+        <v>0.12082912</v>
       </c>
       <c r="P10" s="16">
-        <v>0.1051567239635996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.10515672399999999</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1.5166839999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2681,16 +2768,19 @@
         <v>1305</v>
       </c>
       <c r="N11" s="16">
-        <v>0.77854406130268194</v>
+        <v>0.77394636000000006</v>
       </c>
       <c r="O11" s="16">
-        <v>0.11264367816091954</v>
+        <v>0.112643678</v>
       </c>
       <c r="P11" s="16">
-        <v>0.10881226053639846</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.10881226099999999</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>4.597701E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2731,16 +2821,22 @@
         <v>2366</v>
       </c>
       <c r="N12" s="16">
-        <v>0.79078613693998312</v>
+        <v>0.75612848700000002</v>
       </c>
       <c r="O12" s="16">
-        <v>0.1242603550295858</v>
+        <v>0.124260355</v>
       </c>
       <c r="P12" s="16">
-        <v>8.4953508030431113E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.4953507999999997E-2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>3.4657649999999998E-2</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2781,8 +2877,11 @@
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R13" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2823,16 +2922,19 @@
         <v>3450</v>
       </c>
       <c r="N14" s="16">
-        <v>0.73217391304347823</v>
+        <v>0.71362318800000002</v>
       </c>
       <c r="O14" s="16">
-        <v>0.14840579710144927</v>
+        <v>0.14840579700000001</v>
       </c>
       <c r="P14" s="16">
-        <v>0.11942028985507247</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.11942029</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>1.8550725000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2873,16 +2975,19 @@
         <v>1823</v>
       </c>
       <c r="N15" s="16">
-        <v>0.7153044432254525</v>
+        <v>0.71311025800000005</v>
       </c>
       <c r="O15" s="16">
-        <v>0.17827756445419637</v>
+        <v>0.178277564</v>
       </c>
       <c r="P15" s="16">
-        <v>0.10641799232035107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.106417992</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>2.194185E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2923,16 +3028,19 @@
         <v>1555</v>
       </c>
       <c r="N16" s="16">
-        <v>0.67266881028938907</v>
+        <v>0.67266881000000001</v>
       </c>
       <c r="O16" s="16">
-        <v>0.11639871382636656</v>
+        <v>0.116398714</v>
       </c>
       <c r="P16" s="16">
-        <v>0.21093247588424438</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.21093247600000001</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2973,16 +3081,19 @@
         <v>1724</v>
       </c>
       <c r="N17" s="16">
-        <v>0.62993039443155452</v>
+        <v>0.62819025500000003</v>
       </c>
       <c r="O17" s="16">
-        <v>0.2140371229698376</v>
+        <v>0.214037123</v>
       </c>
       <c r="P17" s="16">
-        <v>0.15603248259860789</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.156032483</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1.7401389999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3023,16 +3134,19 @@
         <v>3197</v>
       </c>
       <c r="N18" s="16">
-        <v>0.79105411323115415</v>
+        <v>0.60212699400000003</v>
       </c>
       <c r="O18" s="16">
-        <v>6.0369096027525805E-2</v>
+        <v>6.0369095999999997E-2</v>
       </c>
       <c r="P18" s="16">
-        <v>0.14857679074131999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.14857679100000001</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.188927119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3074,7 +3188,7 @@
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3115,16 +3229,19 @@
         <v>2125</v>
       </c>
       <c r="N20" s="16">
-        <v>0.64988235294117647</v>
+        <v>0.64705882400000003</v>
       </c>
       <c r="O20" s="16">
-        <v>0.14023529411764707</v>
+        <v>0.14023529400000001</v>
       </c>
       <c r="P20" s="16">
-        <v>0.20988235294117646</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.20988235299999999</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2.823529E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3165,16 +3282,19 @@
         <v>1662</v>
       </c>
       <c r="N21" s="16">
-        <v>0.75932611311672682</v>
+        <v>0.75571600500000002</v>
       </c>
       <c r="O21" s="16">
-        <v>0.15944645006016847</v>
+        <v>0.15944644999999999</v>
       </c>
       <c r="P21" s="16">
-        <v>8.1227436823104696E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.1227437E-2</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>3.6101079999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3215,16 +3335,19 @@
         <v>1936</v>
       </c>
       <c r="N22" s="16">
-        <v>0.92407024793388437</v>
+        <v>0.72727272700000001</v>
       </c>
       <c r="O22" s="16">
-        <v>4.5454545454545456E-2</v>
+        <v>4.5454544999999999E-2</v>
       </c>
       <c r="P22" s="16">
-        <v>3.0475206611570247E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+        <v>3.0475207000000001E-2</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>0.196797521</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3265,16 +3388,19 @@
         <v>3605</v>
       </c>
       <c r="N23" s="16">
-        <v>0.72704576976421642</v>
+        <v>0.72704577000000004</v>
       </c>
       <c r="O23" s="16">
-        <v>0.18335644937586684</v>
+        <v>0.183356449</v>
       </c>
       <c r="P23" s="16">
-        <v>8.9597780859916779E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.9597781000000001E-2</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3316,7 +3442,7 @@
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3357,16 +3483,19 @@
         <v>2131</v>
       </c>
       <c r="N25" s="16">
-        <v>0.78836227123416236</v>
+        <v>0.788362271</v>
       </c>
       <c r="O25" s="16">
-        <v>0.1365556076959174</v>
+        <v>0.13655560799999999</v>
       </c>
       <c r="P25" s="16">
-        <v>7.5082121069920224E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+        <v>7.5082121000000002E-2</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3407,16 +3536,22 @@
         <v>2944</v>
       </c>
       <c r="N26" s="16">
-        <v>0.76358695652173914</v>
+        <v>0.755434783</v>
       </c>
       <c r="O26" s="16">
-        <v>0.16757246376811594</v>
+        <v>0.167572464</v>
       </c>
       <c r="P26" s="16">
-        <v>6.8840579710144928E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.8840579999999998E-2</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>8.1521739999999999E-3</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3457,16 +3592,22 @@
         <v>1472</v>
       </c>
       <c r="N27" s="16">
-        <v>0.76358695652173914</v>
+        <v>0.755434783</v>
       </c>
       <c r="O27" s="16">
-        <v>0.16757246376811594</v>
+        <v>0.167572464</v>
       </c>
       <c r="P27" s="16">
-        <v>6.8840579710144928E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.8840579999999998E-2</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>8.1521739999999999E-3</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3507,16 +3648,19 @@
         <v>1764</v>
       </c>
       <c r="N28" s="16">
-        <v>0.78401360544217691</v>
+        <v>0.70294784600000004</v>
       </c>
       <c r="O28" s="16">
-        <v>8.5034013605442174E-2</v>
+        <v>8.5034014000000005E-2</v>
       </c>
       <c r="P28" s="16">
-        <v>0.13095238095238096</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.13095238100000001</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>8.1065760000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -3557,16 +3701,19 @@
         <v>873</v>
       </c>
       <c r="N29" s="16">
-        <v>0.80641466208476509</v>
+        <v>0.72852233700000002</v>
       </c>
       <c r="O29" s="16">
-        <v>5.2691867124856816E-2</v>
+        <v>5.2691867000000003E-2</v>
       </c>
       <c r="P29" s="16">
-        <v>0.14089347079037801</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.14089347099999999</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>7.7892324999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -3607,16 +3754,19 @@
         <v>1971</v>
       </c>
       <c r="N30" s="16">
-        <v>0.63774733637747349</v>
+        <v>0.59411466300000004</v>
       </c>
       <c r="O30" s="16">
-        <v>0.15677321156773211</v>
+        <v>0.156773212</v>
       </c>
       <c r="P30" s="16">
-        <v>0.20547945205479451</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.20547945200000001</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>4.3632674000000003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -3657,16 +3807,19 @@
         <v>3037</v>
       </c>
       <c r="N31" s="16">
-        <v>0.90286466908133023</v>
+        <v>0.72374053299999996</v>
       </c>
       <c r="O31" s="16">
-        <v>5.6634837010207439E-2</v>
+        <v>5.6634837E-2</v>
       </c>
       <c r="P31" s="16">
-        <v>4.0500493908462297E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+        <v>4.0500493999999998E-2</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>0.17912413599999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -3707,16 +3860,19 @@
         <v>1067</v>
       </c>
       <c r="N32" s="16">
-        <v>0.59418931583880041</v>
+        <v>0.59044048699999996</v>
       </c>
       <c r="O32" s="16">
-        <v>0.25773195876288657</v>
+        <v>0.25773195900000001</v>
       </c>
       <c r="P32" s="16">
-        <v>0.14807872539831302</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.14807872499999999</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>3.7488280000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -3757,16 +3913,19 @@
         <v>4119</v>
       </c>
       <c r="N33" s="16">
-        <v>0.85166302500606939</v>
+        <v>0.76377761600000005</v>
       </c>
       <c r="O33" s="16">
-        <v>0.10900704054382132</v>
+        <v>0.109007041</v>
       </c>
       <c r="P33" s="16">
-        <v>3.9329934450109252E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+        <v>3.9329933999999997E-2</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>8.7885408999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -3808,7 +3967,7 @@
       <c r="O34" s="16"/>
       <c r="P34" s="16"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -3849,16 +4008,19 @@
         <v>1742</v>
       </c>
       <c r="N35" s="16">
-        <v>0.78243398392652119</v>
+        <v>0.774971297</v>
       </c>
       <c r="O35" s="16">
-        <v>0.13260619977037888</v>
+        <v>0.13260620000000001</v>
       </c>
       <c r="P35" s="16">
-        <v>8.4959816303099886E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.4959815999999994E-2</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>7.462687E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -3899,16 +4061,19 @@
         <v>5130</v>
       </c>
       <c r="N36" s="16">
-        <v>0.8267056530214425</v>
+        <v>0.74756335299999999</v>
       </c>
       <c r="O36" s="16">
-        <v>7.2904483430799222E-2</v>
+        <v>7.2904483000000006E-2</v>
       </c>
       <c r="P36" s="16">
-        <v>0.10038986354775828</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.100389864</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>7.9142299999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -3949,8 +4114,11 @@
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
       <c r="P37" s="16"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R37" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -3991,16 +4159,22 @@
         <v>4643</v>
       </c>
       <c r="N38" s="16">
-        <v>0.67973293129442169</v>
+        <v>0.67951755300000005</v>
       </c>
       <c r="O38" s="16">
-        <v>0.12448847727762223</v>
+        <v>0.124488477</v>
       </c>
       <c r="P38" s="16">
-        <v>0.19577859142795606</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.195778591</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>2.1537800000000001E-4</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -4041,16 +4215,19 @@
         <v>3456</v>
       </c>
       <c r="N39" s="16">
-        <v>0.72309027777777779</v>
+        <v>0.69849536999999995</v>
       </c>
       <c r="O39" s="16">
-        <v>0.12210648148148148</v>
+        <v>0.122106481</v>
       </c>
       <c r="P39" s="16">
-        <v>0.15480324074074073</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.15480324100000001</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>2.4594906999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -4091,16 +4268,19 @@
         <v>1235</v>
       </c>
       <c r="N40" s="16">
-        <v>0.63967611336032393</v>
+        <v>0.63967611300000005</v>
       </c>
       <c r="O40" s="16">
-        <v>0.24453441295546557</v>
+        <v>0.24453441300000001</v>
       </c>
       <c r="P40" s="16">
-        <v>0.11578947368421053</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.115789474</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -4141,16 +4321,19 @@
         <v>1143</v>
       </c>
       <c r="N41" s="16">
-        <v>0.84864391951006124</v>
+        <v>0.84601924799999995</v>
       </c>
       <c r="O41" s="16">
-        <v>6.8241469816272965E-2</v>
+        <v>6.8241469999999999E-2</v>
       </c>
       <c r="P41" s="16">
-        <v>8.3114610673665795E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.3114611000000005E-2</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>2.6246720000000002E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -4191,16 +4374,19 @@
         <v>2908</v>
       </c>
       <c r="N42" s="16">
-        <v>0.78129298486932597</v>
+        <v>0.77579092199999999</v>
       </c>
       <c r="O42" s="16">
-        <v>0.11004126547455295</v>
+        <v>0.110041265</v>
       </c>
       <c r="P42" s="16">
-        <v>0.10866574965612105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.10866575000000001</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>5.5020629999999997E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -4241,16 +4427,19 @@
         <v>5130</v>
       </c>
       <c r="N43" s="16">
-        <v>0.8267056530214425</v>
+        <v>0.74756335299999999</v>
       </c>
       <c r="O43" s="16">
-        <v>7.2904483430799222E-2</v>
+        <v>7.2904483000000006E-2</v>
       </c>
       <c r="P43" s="16">
-        <v>0.10038986354775828</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.100389864</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>7.9142299999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -4291,16 +4480,19 @@
         <v>1185</v>
       </c>
       <c r="N44" s="16">
-        <v>0.69620253164556967</v>
+        <v>0.69535864999999997</v>
       </c>
       <c r="O44" s="16">
-        <v>0.16708860759493671</v>
+        <v>0.167088608</v>
       </c>
       <c r="P44" s="16">
-        <v>0.13670886075949368</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.13670886099999999</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>8.4388200000000001E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -4341,16 +4533,19 @@
         <v>2996</v>
       </c>
       <c r="N45" s="16">
-        <v>0.69559412550066757</v>
+        <v>0.69058744999999999</v>
       </c>
       <c r="O45" s="16">
-        <v>0.16555407209612816</v>
+        <v>0.165554072</v>
       </c>
       <c r="P45" s="16">
-        <v>0.13885180240320427</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.138851802</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>5.0066759999999998E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -4391,16 +4586,19 @@
         <v>2539</v>
       </c>
       <c r="N46" s="16">
-        <v>0.80661677825915712</v>
+        <v>0.80582906700000001</v>
       </c>
       <c r="O46" s="16">
-        <v>0.12012603387160299</v>
+        <v>0.12012603400000001</v>
       </c>
       <c r="P46" s="16">
-        <v>7.3257187869239862E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+        <v>7.3257188000000001E-2</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>7.8771199999999998E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -4441,16 +4639,19 @@
         <v>2097</v>
       </c>
       <c r="N47" s="16">
-        <v>0.66046733428707682</v>
+        <v>0.63567000500000004</v>
       </c>
       <c r="O47" s="16">
-        <v>0.10348116356700048</v>
+        <v>0.103481164</v>
       </c>
       <c r="P47" s="16">
-        <v>0.23605150214592274</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.236051502</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>2.4797329999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -4491,16 +4692,19 @@
         <v>3189</v>
       </c>
       <c r="N48" s="16">
-        <v>0.66509877704609599</v>
+        <v>0.66259015399999999</v>
       </c>
       <c r="O48" s="16">
-        <v>0.11571025399811853</v>
+        <v>0.115710254</v>
       </c>
       <c r="P48" s="16">
-        <v>0.21919096895578552</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.21919096900000001</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>2.5086230000000002E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -4541,16 +4745,19 @@
         <v>4793</v>
       </c>
       <c r="N49" s="16">
-        <v>0.77842687252242848</v>
+        <v>0.77279365700000002</v>
       </c>
       <c r="O49" s="16">
-        <v>9.4721468808679321E-2</v>
+        <v>9.4721469000000003E-2</v>
       </c>
       <c r="P49" s="16">
-        <v>0.12685165866889214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.12685165900000001</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>5.6332149999999996E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -4591,16 +4798,19 @@
         <v>1222</v>
       </c>
       <c r="N50" s="16">
-        <v>0.67021276595744683</v>
+        <v>0.67021276600000002</v>
       </c>
       <c r="O50" s="16">
-        <v>0.13011456628477905</v>
+        <v>0.13011456599999999</v>
       </c>
       <c r="P50" s="16">
-        <v>0.19967266775777415</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.199672668</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -4641,16 +4851,22 @@
         <v>2729.6</v>
       </c>
       <c r="N51" s="16">
-        <v>0.73036342321219228</v>
+        <v>0.72919109000000004</v>
       </c>
       <c r="O51" s="16">
-        <v>0.11400937866354044</v>
+        <v>0.11400937899999999</v>
       </c>
       <c r="P51" s="16">
-        <v>0.15562719812426731</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.15562719799999999</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>1.172333E-3</v>
+      </c>
+      <c r="R51" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -4691,16 +4907,22 @@
         <v>682.4</v>
       </c>
       <c r="N52" s="16">
-        <v>0.73036342321219228</v>
+        <v>0.72919109000000004</v>
       </c>
       <c r="O52" s="16">
-        <v>0.11400937866354044</v>
+        <v>0.11400937899999999</v>
       </c>
       <c r="P52" s="16">
-        <v>0.15562719812426731</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.15562719799999999</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>1.172333E-3</v>
+      </c>
+      <c r="R52" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>51</v>
       </c>
@@ -4741,16 +4963,22 @@
         <v>3929</v>
       </c>
       <c r="N53" s="16">
-        <v>0.78849580045813172</v>
+        <v>0.62458640899999995</v>
       </c>
       <c r="O53" s="16">
-        <v>0.11300585390684653</v>
+        <v>0.113005854</v>
       </c>
       <c r="P53" s="16">
-        <v>9.8498345635021634E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+        <v>9.8498346000000001E-2</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>0.16390939199999999</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -4791,16 +5019,22 @@
         <v>3559</v>
       </c>
       <c r="N54" s="16">
-        <v>0.83675189660016858</v>
+        <v>0.81005900500000005</v>
       </c>
       <c r="O54" s="16">
-        <v>5.4790671536948582E-2</v>
+        <v>5.4790671999999999E-2</v>
       </c>
       <c r="P54" s="16">
-        <v>0.10845743186288283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.10845743200000001</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>2.6692891E-2</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -4841,16 +5075,19 @@
         <v>786</v>
       </c>
       <c r="N55" s="16">
-        <v>0.70356234096692116</v>
+        <v>0.70356234100000004</v>
       </c>
       <c r="O55" s="16">
-        <v>0.17302798982188294</v>
+        <v>0.17302798999999999</v>
       </c>
       <c r="P55" s="16">
-        <v>0.12340966921119594</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.123409669</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -4891,16 +5128,19 @@
         <v>3450</v>
       </c>
       <c r="N56" s="16">
-        <v>0.73217391304347823</v>
+        <v>0.71362318800000002</v>
       </c>
       <c r="O56" s="16">
-        <v>0.14840579710144927</v>
+        <v>0.14840579700000001</v>
       </c>
       <c r="P56" s="16">
-        <v>0.11942028985507247</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.11942029</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>1.8550725000000001E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -4941,16 +5181,19 @@
         <v>2908</v>
       </c>
       <c r="N57" s="16">
-        <v>0.74381017881705636</v>
+        <v>0.73349381000000002</v>
       </c>
       <c r="O57" s="16">
-        <v>0.15061898211829436</v>
+        <v>0.15061898200000001</v>
       </c>
       <c r="P57" s="16">
-        <v>0.10557083906464924</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.105570839</v>
+      </c>
+      <c r="Q57" s="2">
+        <v>1.0316369000000001E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>56</v>
       </c>
@@ -4991,16 +5234,19 @@
         <v>3096</v>
       </c>
       <c r="N58" s="16">
-        <v>0.71447028423772607</v>
+        <v>0.71156330700000003</v>
       </c>
       <c r="O58" s="16">
-        <v>0.16957364341085271</v>
+        <v>0.169573643</v>
       </c>
       <c r="P58" s="16">
-        <v>0.11595607235142119</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.11595607199999999</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>2.9069769999999998E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>57</v>
       </c>
@@ -5041,16 +5287,19 @@
         <v>1708</v>
       </c>
       <c r="N59" s="16">
-        <v>0.63056206088992972</v>
+        <v>0.62939110099999995</v>
       </c>
       <c r="O59" s="16">
-        <v>0.13466042154566746</v>
+        <v>0.134660422</v>
       </c>
       <c r="P59" s="16">
-        <v>0.23477751756440282</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.23477751799999999</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>1.17096E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -5091,16 +5340,19 @@
         <v>1372</v>
       </c>
       <c r="N60" s="16">
-        <v>0.70189504373177847</v>
+        <v>0.70189504400000002</v>
       </c>
       <c r="O60" s="16">
-        <v>0.17055393586005832</v>
+        <v>0.17055393599999999</v>
       </c>
       <c r="P60" s="16">
-        <v>0.12755102040816327</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.12755101999999999</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -5141,16 +5393,19 @@
         <v>776</v>
       </c>
       <c r="N61" s="16">
-        <v>0.759020618556701</v>
+        <v>0.75902061899999995</v>
       </c>
       <c r="O61" s="16">
-        <v>0.11211340206185567</v>
+        <v>0.112113402</v>
       </c>
       <c r="P61" s="16">
-        <v>0.12886597938144329</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.12886597899999999</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -5191,16 +5446,19 @@
         <v>1327</v>
       </c>
       <c r="N62" s="16">
-        <v>0.75131876412961573</v>
+        <v>0.75056518500000002</v>
       </c>
       <c r="O62" s="16">
-        <v>0.13187641296156744</v>
+        <v>0.131876413</v>
       </c>
       <c r="P62" s="16">
-        <v>0.11680482290881689</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.116804823</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>7.5358000000000001E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -5242,7 +5500,7 @@
       <c r="O63" s="16"/>
       <c r="P63" s="16"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -5283,16 +5541,19 @@
         <v>3840</v>
       </c>
       <c r="N64" s="16">
-        <v>0.75390625</v>
+        <v>0.703125</v>
       </c>
       <c r="O64" s="16">
-        <v>0.12005208333333334</v>
+        <v>0.120052083</v>
       </c>
       <c r="P64" s="16">
-        <v>0.12604166666666666</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.126041667</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>5.078125E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -5334,7 +5595,7 @@
       <c r="O65" s="16"/>
       <c r="P65" s="16"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -5375,16 +5636,19 @@
         <v>939</v>
       </c>
       <c r="N66" s="16">
-        <v>0.74334398296059634</v>
+        <v>0.76677316299999998</v>
       </c>
       <c r="O66" s="16">
-        <v>0.16080937167199147</v>
+        <v>0.16080937200000001</v>
       </c>
       <c r="P66" s="16">
-        <v>9.5846645367412137E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+        <v>9.5846644999999994E-2</v>
+      </c>
+      <c r="Q66" s="2">
+        <v>-2.3429180000000001E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -5425,8 +5689,11 @@
       <c r="N67" s="16"/>
       <c r="O67" s="16"/>
       <c r="P67" s="16"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R67" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -5467,16 +5734,22 @@
         <v>4320</v>
       </c>
       <c r="N68" s="16">
-        <v>0.77361111111111114</v>
+        <v>0.73634259300000005</v>
       </c>
       <c r="O68" s="16">
-        <v>0.11435185185185186</v>
+        <v>0.114351852</v>
       </c>
       <c r="P68" s="16">
-        <v>0.11203703703703703</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.11203703700000001</v>
+      </c>
+      <c r="Q68" s="2">
+        <v>3.7268519E-2</v>
+      </c>
+      <c r="R68" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>67</v>
       </c>
@@ -5517,16 +5790,19 @@
         <v>737</v>
       </c>
       <c r="N69" s="16">
-        <v>0.78018995929443702</v>
+        <v>0.81953867000000002</v>
       </c>
       <c r="O69" s="16">
-        <v>0.12347354138398914</v>
+        <v>0.12347354100000001</v>
       </c>
       <c r="P69" s="16">
-        <v>9.6336499321573954E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+        <v>9.6336499000000006E-2</v>
+      </c>
+      <c r="Q69" s="2">
+        <v>-3.9348711000000001E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>68</v>
       </c>
@@ -5567,16 +5843,19 @@
         <v>939</v>
       </c>
       <c r="N70" s="16">
-        <v>0.6911608093716719</v>
+        <v>0.69009584700000004</v>
       </c>
       <c r="O70" s="16">
-        <v>0.13844515441959532</v>
+        <v>0.13844515399999999</v>
       </c>
       <c r="P70" s="16">
-        <v>0.1703940362087327</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.170394036</v>
+      </c>
+      <c r="Q70" s="2">
+        <v>1.0649629999999999E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>69</v>
       </c>
@@ -5617,16 +5896,22 @@
         <v>2316</v>
       </c>
       <c r="N71" s="16">
-        <v>0.66018998272884288</v>
+        <v>0.65975820399999996</v>
       </c>
       <c r="O71" s="16">
-        <v>0.2189119170984456</v>
+        <v>0.21891191700000001</v>
       </c>
       <c r="P71" s="16">
-        <v>0.12089810017271158</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.12089809999999999</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>4.3177899999999997E-4</v>
+      </c>
+      <c r="R71" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -5667,8 +5952,11 @@
       <c r="N72" s="16"/>
       <c r="O72" s="16"/>
       <c r="P72" s="16"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R72" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -5709,8 +5997,11 @@
       <c r="N73" s="16"/>
       <c r="O73" s="16"/>
       <c r="P73" s="16"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R73" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -5751,8 +6042,11 @@
       <c r="N74" s="16"/>
       <c r="O74" s="16"/>
       <c r="P74" s="16"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R74" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -5793,16 +6087,22 @@
         <v>1212</v>
       </c>
       <c r="N75" s="16">
-        <v>0.75165016501650161</v>
+        <v>0.74669967000000004</v>
       </c>
       <c r="O75" s="16">
-        <v>0.1476897689768977</v>
+        <v>0.147689769</v>
       </c>
       <c r="P75" s="16">
-        <v>0.10066006600660066</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.10066006600000001</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>4.9504950000000001E-3</v>
+      </c>
+      <c r="R75" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -5843,16 +6143,19 @@
         <v>2032</v>
       </c>
       <c r="N76" s="16">
-        <v>0.7514763779527559</v>
+        <v>0.74655511799999996</v>
       </c>
       <c r="O76" s="16">
-        <v>0.11515748031496063</v>
+        <v>0.11515748000000001</v>
       </c>
       <c r="P76" s="16">
-        <v>0.13336614173228348</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.13336614199999999</v>
+      </c>
+      <c r="Q76" s="2">
+        <v>4.9212600000000002E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -5893,8 +6196,11 @@
       <c r="N77" s="16"/>
       <c r="O77" s="16"/>
       <c r="P77" s="16"/>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R77" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -5935,16 +6241,22 @@
         <v>2884</v>
       </c>
       <c r="N78" s="16">
-        <v>0.76248266296809986</v>
+        <v>0.75312066600000005</v>
       </c>
       <c r="O78" s="16">
-        <v>0.17649098474341193</v>
+        <v>0.17649098499999999</v>
       </c>
       <c r="P78" s="16">
-        <v>6.1026352288488211E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.1026351999999999E-2</v>
+      </c>
+      <c r="Q78" s="2">
+        <v>9.3619970000000004E-3</v>
+      </c>
+      <c r="R78" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -5985,16 +6297,19 @@
         <v>1467</v>
       </c>
       <c r="N79" s="16">
-        <v>0.74778459441036127</v>
+        <v>0.74028629899999998</v>
       </c>
       <c r="O79" s="16">
-        <v>0.1492842535787321</v>
+        <v>0.14928425400000001</v>
       </c>
       <c r="P79" s="16">
-        <v>0.10293115201090661</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.102931152</v>
+      </c>
+      <c r="Q79" s="2">
+        <v>7.4982959999999998E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -6035,16 +6350,19 @@
         <v>1695</v>
       </c>
       <c r="N80" s="16">
-        <v>0.87197640117994102</v>
+        <v>0.86489675499999996</v>
       </c>
       <c r="O80" s="16">
-        <v>6.2536873156342182E-2</v>
+        <v>6.2536873000000007E-2</v>
       </c>
       <c r="P80" s="16">
-        <v>6.5486725663716813E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+        <v>6.5486725999999995E-2</v>
+      </c>
+      <c r="Q80" s="2">
+        <v>7.0796460000000002E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -6085,16 +6403,19 @@
         <v>988</v>
       </c>
       <c r="N81" s="16">
-        <v>0.74898785425101211</v>
+        <v>0.74898785400000001</v>
       </c>
       <c r="O81" s="16">
-        <v>0.11437246963562753</v>
+        <v>0.11437247</v>
       </c>
       <c r="P81" s="16">
-        <v>0.13663967611336034</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.13663967599999999</v>
+      </c>
+      <c r="Q81" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>80</v>
       </c>
@@ -6135,16 +6456,19 @@
         <v>1599</v>
       </c>
       <c r="N82" s="16">
-        <v>0.75984990619136961</v>
+        <v>0.73170731700000002</v>
       </c>
       <c r="O82" s="16">
-        <v>0.13195747342088807</v>
+        <v>0.13195747299999999</v>
       </c>
       <c r="P82" s="16">
-        <v>0.10819262038774234</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.10819262</v>
+      </c>
+      <c r="Q82" s="2">
+        <v>2.8142588999999999E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -6185,16 +6509,19 @@
         <v>1361</v>
       </c>
       <c r="N83" s="16">
-        <v>0.72446730345334309</v>
+        <v>0.72446730299999995</v>
       </c>
       <c r="O83" s="16">
-        <v>0.1807494489346069</v>
+        <v>0.18074944900000001</v>
       </c>
       <c r="P83" s="16">
-        <v>9.4783247612049967E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+        <v>9.4783248E-2</v>
+      </c>
+      <c r="Q83" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -6235,16 +6562,19 @@
         <v>3037</v>
       </c>
       <c r="N84" s="16">
-        <v>0.60059269015475802</v>
+        <v>0.59762923899999998</v>
       </c>
       <c r="O84" s="16">
-        <v>0.112940401712216</v>
+        <v>0.112940402</v>
       </c>
       <c r="P84" s="16">
-        <v>0.286466908133026</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.28646690800000002</v>
+      </c>
+      <c r="Q84" s="2">
+        <v>2.9634510000000002E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -6285,16 +6615,19 @@
         <v>1378</v>
       </c>
       <c r="N85" s="16">
-        <v>0.67489114658925975</v>
+        <v>0.67053700999999999</v>
       </c>
       <c r="O85" s="16">
-        <v>0.1204644412191582</v>
+        <v>0.12046444100000001</v>
       </c>
       <c r="P85" s="16">
-        <v>0.204644412191582</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.204644412</v>
+      </c>
+      <c r="Q85" s="2">
+        <v>4.3541359999999998E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -6335,16 +6668,22 @@
         <v>1898</v>
       </c>
       <c r="N86" s="16">
-        <v>0.71601685985247621</v>
+        <v>0.63382507899999996</v>
       </c>
       <c r="O86" s="16">
-        <v>3.3192834562697573E-2</v>
+        <v>3.3192834999999997E-2</v>
       </c>
       <c r="P86" s="16">
-        <v>0.25079030558482612</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.25079030600000002</v>
+      </c>
+      <c r="Q86" s="2">
+        <v>8.2191781000000005E-2</v>
+      </c>
+      <c r="R86" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -6385,16 +6724,19 @@
         <v>4793</v>
       </c>
       <c r="N87" s="16">
-        <v>0.77842687252242848</v>
+        <v>0.77279365700000002</v>
       </c>
       <c r="O87" s="16">
-        <v>9.4721468808679321E-2</v>
+        <v>9.4721469000000003E-2</v>
       </c>
       <c r="P87" s="16">
-        <v>0.12685165866889214</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+        <v>0.12685165900000001</v>
+      </c>
+      <c r="Q87" s="2">
+        <v>5.6332149999999996E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -6435,16 +6777,19 @@
         <v>671</v>
       </c>
       <c r="N88" s="16">
-        <v>0.77794336810730258</v>
+        <v>0.77496274200000004</v>
       </c>
       <c r="O88" s="16">
-        <v>0.20268256333830104</v>
+        <v>0.20268256300000001</v>
       </c>
       <c r="P88" s="16">
-        <v>1.9374068554396422E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+        <v>1.9374069000000001E-2</v>
+      </c>
+      <c r="Q88" s="2">
+        <v>2.9806260000000001E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -6485,16 +6830,22 @@
         <v>2751</v>
       </c>
       <c r="N89" s="16">
-        <v>0.83133406034169399</v>
+        <v>0.829516539</v>
       </c>
       <c r="O89" s="16">
-        <v>8.8331515812431843E-2</v>
+        <v>8.8331515999999999E-2</v>
       </c>
       <c r="P89" s="16">
-        <v>8.0334423845874234E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+        <v>8.0334424000000001E-2</v>
+      </c>
+      <c r="Q89" s="2">
+        <v>1.8175209999999999E-3</v>
+      </c>
+      <c r="R89" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -6535,23 +6886,26 @@
       <c r="N90" s="16"/>
       <c r="O90" s="16"/>
       <c r="P90" s="16"/>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R90" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M91" s="18"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M92" s="18"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M93" s="18"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M94" s="18"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M95" s="18"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M96" s="18"/>
     </row>
     <row r="97" spans="13:13" x14ac:dyDescent="0.3">

</xml_diff>